<commit_message>
Fix some error in practice 05
</commit_message>
<xml_diff>
--- a/Excel动手实验室 - 材料/05 - 自动填充和快速填充.xlsx
+++ b/Excel动手实验室 - 材料/05 - 自动填充和快速填充.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="5055"/>
+    <workbookView xWindow="0" yWindow="347" windowWidth="14460" windowHeight="5051"/>
   </bookViews>
   <sheets>
     <sheet name="简介" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>Nancy.Freehafer@fourthcoffee.com</t>
   </si>
@@ -302,46 +302,6 @@
   </si>
   <si>
     <t>姓氏</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>51010619860203610</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>51010619880508610</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>51010619880509610</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>51010619860103610</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>51010619810508610</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>51010619830203610</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>身份证号</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>51010619820518610</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>51010619790728610</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>51010619771218610</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -350,13 +310,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -364,14 +324,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -511,7 +471,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -524,7 +484,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="32" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -551,16 +511,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
@@ -578,15 +535,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -962,117 +910,117 @@
   <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="3" max="3" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.25">
+    <row r="3" spans="1:4" ht="15.45">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="14.25">
+    <row r="4" spans="1:4" ht="15.45">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="14.25">
+    <row r="5" spans="1:4" ht="15.45">
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" ht="14.25">
+    <row r="6" spans="1:4" ht="15.45">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="14.25">
+    <row r="7" spans="1:4" ht="15.45">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" ht="14.25">
+    <row r="8" spans="1:4" ht="15.45">
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="14.25">
+    <row r="9" spans="1:4" ht="15.45">
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="14.25">
+    <row r="10" spans="1:4" ht="15.45">
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="14.25">
+    <row r="11" spans="1:4" ht="15.45">
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="14.25">
+    <row r="12" spans="1:4" ht="15.45">
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="14.25">
+    <row r="13" spans="1:4" ht="15.45">
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="14.25">
+    <row r="14" spans="1:4" ht="15.45">
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="14.25">
+    <row r="15" spans="1:4" ht="15.45">
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="14.25">
+    <row r="16" spans="1:4" ht="15.45">
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="3:4" ht="14.25">
+    <row r="17" spans="3:4" ht="15.45">
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="3:4" ht="14.25">
+    <row r="18" spans="3:4" ht="15.45">
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1092,14 +1040,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="8.375" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="8.3984375" customWidth="1"/>
+    <col min="7" max="7" width="12.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1188,16 +1138,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="12.46484375" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
-    <col min="5" max="5" width="14.625" customWidth="1"/>
-    <col min="7" max="7" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" customWidth="1"/>
+    <col min="5" max="5" width="14.59765625" customWidth="1"/>
+    <col min="7" max="7" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1215,10 +1167,10 @@
         <v>13612340001</v>
       </c>
       <c r="B2" s="10"/>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <v>19610221</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1227,90 +1179,90 @@
         <v>13712342467</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>19661202</v>
       </c>
-      <c r="E3" s="18"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8">
         <v>15112342551</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>19641019</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8">
         <v>15212346834</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>19740527</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8">
         <v>15312345839</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>19730304</v>
       </c>
-      <c r="E6" s="18"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="8">
         <v>18912346749</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>19430728</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="8">
         <v>15012348307</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>19640316</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="8">
         <v>15312346720</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>19480223</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8">
         <v>17012348735</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>19731208</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="9">
         <v>17112341659</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <v>19800311</v>
       </c>
-      <c r="E11" s="19"/>
+      <c r="E11" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1320,18 +1272,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.46484375" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1342,21 +1295,17 @@
         <v>38</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
         <v>39</v>
       </c>
@@ -1372,12 +1321,8 @@
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
-      <c r="J2" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="13"/>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>42</v>
       </c>
@@ -1393,12 +1338,8 @@
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="J3" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>45</v>
       </c>
@@ -1412,12 +1353,8 @@
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="J4" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="8" t="s">
         <v>47</v>
       </c>
@@ -1433,12 +1370,8 @@
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="J5" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
         <v>50</v>
       </c>
@@ -1454,12 +1387,8 @@
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
-      <c r="J6" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="8" t="s">
         <v>53</v>
       </c>
@@ -1473,12 +1402,8 @@
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="J7" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
         <v>55</v>
       </c>
@@ -1494,12 +1419,8 @@
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="J8" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
         <v>58</v>
       </c>
@@ -1515,12 +1436,8 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="J9" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:11">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="9" t="s">
         <v>61</v>
       </c>
@@ -1536,10 +1453,6 @@
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
-      <c r="J10" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>